<commit_message>
Error message is red, more clarity on tooltip text
</commit_message>
<xml_diff>
--- a/test/good_dyns/excel/test.xlsx
+++ b/test/good_dyns/excel/test.xlsx
@@ -7,41 +7,45 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet34" sheetId="35" r:id="rId1"/>
-    <sheet name="Sheet33" sheetId="34" r:id="rId2"/>
-    <sheet name="Sheet32" sheetId="33" r:id="rId3"/>
-    <sheet name="Sheet31" sheetId="32" r:id="rId4"/>
-    <sheet name="Sheet30" sheetId="31" r:id="rId5"/>
-    <sheet name="Sheet29" sheetId="30" r:id="rId6"/>
-    <sheet name="Sheet28" sheetId="29" r:id="rId7"/>
-    <sheet name="Sheet27" sheetId="28" r:id="rId8"/>
-    <sheet name="Sheet26" sheetId="27" r:id="rId9"/>
-    <sheet name="Sheet25" sheetId="26" r:id="rId10"/>
-    <sheet name="Sheet24" sheetId="25" r:id="rId11"/>
-    <sheet name="Sheet23" sheetId="24" r:id="rId12"/>
-    <sheet name="Sheet22" sheetId="23" r:id="rId13"/>
-    <sheet name="Sheet21" sheetId="22" r:id="rId14"/>
-    <sheet name="Sheet20" sheetId="21" r:id="rId15"/>
-    <sheet name="Sheet19" sheetId="20" r:id="rId16"/>
-    <sheet name="Sheet18" sheetId="19" r:id="rId17"/>
-    <sheet name="Sheet17" sheetId="18" r:id="rId18"/>
-    <sheet name="Sheet16" sheetId="17" r:id="rId19"/>
-    <sheet name="Sheet15" sheetId="16" r:id="rId20"/>
-    <sheet name="Sheet14" sheetId="15" r:id="rId21"/>
-    <sheet name="Sheet13" sheetId="14" r:id="rId22"/>
-    <sheet name="Sheet12" sheetId="13" r:id="rId23"/>
-    <sheet name="Sheet11" sheetId="12" r:id="rId24"/>
-    <sheet name="Sheet10" sheetId="11" r:id="rId25"/>
-    <sheet name="Sheet9" sheetId="10" r:id="rId26"/>
-    <sheet name="Sheet8" sheetId="9" r:id="rId27"/>
-    <sheet name="Sheet7" sheetId="8" r:id="rId28"/>
-    <sheet name="Sheet6" sheetId="7" r:id="rId29"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId30"/>
-    <sheet name="Pedro" sheetId="5" r:id="rId31"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId32"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId33"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId34"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId35"/>
+    <sheet name="Sheet38" sheetId="39" r:id="rId1"/>
+    <sheet name="Sheet37" sheetId="38" r:id="rId2"/>
+    <sheet name="Sheet36" sheetId="37" r:id="rId3"/>
+    <sheet name="Sheet35" sheetId="36" r:id="rId4"/>
+    <sheet name="Sheet34" sheetId="35" r:id="rId5"/>
+    <sheet name="Sheet33" sheetId="34" r:id="rId6"/>
+    <sheet name="Sheet32" sheetId="33" r:id="rId7"/>
+    <sheet name="Sheet31" sheetId="32" r:id="rId8"/>
+    <sheet name="Sheet30" sheetId="31" r:id="rId9"/>
+    <sheet name="Sheet29" sheetId="30" r:id="rId10"/>
+    <sheet name="Sheet28" sheetId="29" r:id="rId11"/>
+    <sheet name="Sheet27" sheetId="28" r:id="rId12"/>
+    <sheet name="Sheet26" sheetId="27" r:id="rId13"/>
+    <sheet name="Sheet25" sheetId="26" r:id="rId14"/>
+    <sheet name="Sheet24" sheetId="25" r:id="rId15"/>
+    <sheet name="Sheet23" sheetId="24" r:id="rId16"/>
+    <sheet name="Sheet22" sheetId="23" r:id="rId17"/>
+    <sheet name="Sheet21" sheetId="22" r:id="rId18"/>
+    <sheet name="Sheet20" sheetId="21" r:id="rId19"/>
+    <sheet name="Sheet19" sheetId="20" r:id="rId20"/>
+    <sheet name="Sheet18" sheetId="19" r:id="rId21"/>
+    <sheet name="Sheet17" sheetId="18" r:id="rId22"/>
+    <sheet name="Sheet16" sheetId="17" r:id="rId23"/>
+    <sheet name="Sheet15" sheetId="16" r:id="rId24"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId25"/>
+    <sheet name="Sheet13" sheetId="14" r:id="rId26"/>
+    <sheet name="Sheet12" sheetId="13" r:id="rId27"/>
+    <sheet name="Sheet11" sheetId="12" r:id="rId28"/>
+    <sheet name="Sheet10" sheetId="11" r:id="rId29"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId30"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId31"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId32"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId33"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId34"/>
+    <sheet name="Pedro" sheetId="5" r:id="rId35"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId36"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId37"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId38"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId39"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -422,18 +426,6 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -450,103 +442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4"/>
   <sheetViews>
@@ -564,55 +460,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4"/>
   <sheetViews>
@@ -630,43 +514,103 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4"/>
   <sheetViews>
@@ -684,31 +628,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4"/>
   <sheetViews>
@@ -726,7 +694,103 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -763,31 +827,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -800,6 +864,54 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4"/>
   <sheetViews>
@@ -817,66 +929,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>

</xml_diff>